<commit_message>
qr like image and link in table
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="662">
   <si>
     <t>Date</t>
   </si>
@@ -67,7 +67,7 @@
     <t>HDLO+6gqDKL6E1jY/yWe9Hplo2WEmku01/xcGjkY9NVTEr68XT2ZpqZF91a1D9JbnKkJg1UuljvPQDEfKRYAitM=</t>
   </si>
   <si>
-    <t>certificate_Петро_Петрович_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1NIP-hUzOdK687sr_-NrbAOJYvlB-VJva/view</t>
   </si>
   <si>
     <t>10.05.2016</t>
@@ -88,7 +88,7 @@
     <t>HL/S5ow1QPozfKwI1cDRfp+h8sLtxXuxGlTDhhX9Rk8OYiSML1LOd3RwysGcf0ZTK3oLyrYpOiW7SgN6uB2ZYGE=</t>
   </si>
   <si>
-    <t>certificate_Nikita_Magda_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1F5yp9xvcd06Fh2nyypzqmfayeNW83BLQ/view</t>
   </si>
   <si>
     <t>Нестеров Максим</t>
@@ -103,7 +103,7 @@
     <t>HLC5z4t8xC2YGKI5mLBpvDsQ3DOM3PbbILeTlOKwjBm4K0esTGfEknzQuCJ2yEB6ovYnuMtL+MmBHQck4r/Og7Q=</t>
   </si>
   <si>
-    <t>certificate_Нестеров_Максим_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1NGhSv13MDtbBCPSQwz6m8ztAZWlHgtxs/view</t>
   </si>
   <si>
     <t>Alexey Shendrick</t>
@@ -118,7 +118,7 @@
     <t>G68tQOmxtEYSkwR0sAY0ML8dBFo2Wi5mIbiy/fK07in9KXs9kunnFY/GlAbA/kda8OlqjC0Lk97BBUjUuPnTpHk=</t>
   </si>
   <si>
-    <t>certificate_Alexey_Shendrick_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1xPM2g224BtkOQ1Nx4-YsqntUthOJ1Huu/view</t>
   </si>
   <si>
     <t>Anastasia Sapozhkova</t>
@@ -133,7 +133,7 @@
     <t>HK6wLdEeplEYXJCkmuaJlVdEHn86MGUCs4DDpbEd93LNV2ZF6etTLCUq6k5abJlgfDVKnjx9yOW4QN5HVbwJDj4=</t>
   </si>
   <si>
-    <t>certificate_Anastasia_Sapozhkova_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1PuvaE-mDyRPmV3yXCj4rgzc_WSlO9Y0F/view</t>
   </si>
   <si>
     <t>Den Galkin</t>
@@ -148,7 +148,7 @@
     <t>GzNRug/B6l+rL3to9AZ/VXpmusTsWvucAR9DOc2FTvxrM93KfyaXy/tA1JNI2m3n6U6h0HTVd5LDJ42ktB0U0wI=</t>
   </si>
   <si>
-    <t>certificate_Den_Galkin_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1ZlwGSZlDffX3T6gyLAKlwRbfmy76qvO4/view</t>
   </si>
   <si>
     <t>Daniyil Yakovlev</t>
@@ -163,7 +163,7 @@
     <t>G/OqvWSw7yJjGNtQrDOgmqM+KDGFPtg2ik0kjJI3j4VcUnwk8Er+CGUs7gv6f0fzp9aYI8HWFOe1JYwKeX4iB9o=</t>
   </si>
   <si>
-    <t>certificate_Daniyil_Yakovlev_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1CX7yKhFFJESfkrB2rrNdzpYtWpB0kltD/view</t>
   </si>
   <si>
     <t>Алексей Демидов</t>
@@ -178,7 +178,7 @@
     <t>HFwp//oNPDU4M9oHCqEUpLHoBO+T79UoW0yCBU00B7CAaH3b/yUVFO8KZd020njZS2MqV8d4gU92CV7PwMy3l6Q=</t>
   </si>
   <si>
-    <t>certificate_Алексей_Демидов_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1TrseCsDonCJM5ByZH6AYc6hFQMJO8RzK/view</t>
   </si>
   <si>
     <t>Анатолий Дедов</t>
@@ -193,7 +193,7 @@
     <t>G1pZdlCrJdkeNY36bRW+19+z8QM+FB5hoRGkvwdbEQkzYjL8dY0VCVAEzrHmA0RjSxDq8sPPcBb0z7gDyiSNUMQ=</t>
   </si>
   <si>
-    <t>certificate_Анатолий_Дедов_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1ETsgJL_wSHAJYaVOMJ66ceO-PhS_0dJc/view</t>
   </si>
   <si>
     <t>Денис Руденко</t>
@@ -208,7 +208,7 @@
     <t>HOuQkxXy/PqMOZJFmEUoMQk95GdnTEdDxzlbCmyKlOZmDvKXPg/DKRRZ4kEEvI30D+swVXxp4x8eKy1TYChtps8=</t>
   </si>
   <si>
-    <t>certificate_Денис_Руденко_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/11euEe_QfLkLGeofABp4JMNUzl6Ka0m_s/view</t>
   </si>
   <si>
     <t>Illia Fariatiev</t>
@@ -223,7 +223,7 @@
     <t>G1RRBhBcOU6M8nvMrq1O5P7aq2wiUecvqkXw/SoQk+GOLYc0oML5nQiOMrDAiM90Q67nNRLBMjlL8RfqtQngLZ8=</t>
   </si>
   <si>
-    <t>certificate_Illia_Fariatiev_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1ZT5FFBG33BeM8R0Z4z5mCszVi3u1xwKC/view</t>
   </si>
   <si>
     <t>Костюк Александр</t>
@@ -238,7 +238,7 @@
     <t>G6l/nUfobqeYO+SaS/PyhLMSJWjouG2QrzL8m9JyLZPmdXpYmDUXWPL30/Vaz60KIPhLXWqj6JP2YoqtYXmpn9k=</t>
   </si>
   <si>
-    <t>certificate_Костюк_Александр_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1v--jgEX3TUrEHx2jUFNHVwWGgVvkjBOI/view</t>
   </si>
   <si>
     <t>Марина Боровая</t>
@@ -253,7 +253,7 @@
     <t>G3CfLZYX4HzXNNASC36O1805sLJKVdL2UWzcwOt1+J+mZwe+2/x49eTPU3e2hdytEDtjniiqAqXtnUEL+7EEyVM=</t>
   </si>
   <si>
-    <t>certificate_Марина_Боровая_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/123vvGb-L-2OL46dMID8eLhGmy9Fu2L4n/view</t>
   </si>
   <si>
     <t>Мордвинов Роман Игоревич</t>
@@ -268,7 +268,7 @@
     <t>G3+B366TAXptnN3HvQySms9KyzVyfDsYIXw3O8Lw3Q6DdbZU0hTkIcnc0CTYsgjyxaTjGqf+1uDrdEWWYpXgpc4=</t>
   </si>
   <si>
-    <t>certificate_Мордвинов_Роман_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1kBEQXPEfiNu95-c8tcN8ISSUI2yynUwD/view</t>
   </si>
   <si>
     <t>Сергей Романько</t>
@@ -283,7 +283,7 @@
     <t>G4Jpj2CKvbUWopbxx+r1S4P4a00i1vVFiWxaDaid3qXMd+O3iUkAcnZLIXUHDkeeObPXvwnDyWfVdP81UEiVhN8=</t>
   </si>
   <si>
-    <t>certificate_Сергей_Романько_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1OUXMxR-gnY9VPJcschk5LEBNEpnXQN67/view</t>
   </si>
   <si>
     <t>Синельников Александр</t>
@@ -298,7 +298,7 @@
     <t>G5UswIvpVEAXG7zWhMchCB6uvXSRacPk9rNvBDGtXpCjMRkXkOvyNsz3nz5I+OHrYByOypWdRVomNhRH7wBxt98=</t>
   </si>
   <si>
-    <t>certificate_Синельников_Александр_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1ThzYFALLWsSe0fZRdMlGIBXJiXOPUcNq/view</t>
   </si>
   <si>
     <t>Скрипник Александр</t>
@@ -313,7 +313,7 @@
     <t>G4JMoj4xVjoSztKT0vJkm89W+TB3IA5K/94xv0+kLibqblxl3tfwpnqbdoeMFikP+MhqLYT3ik6COvUNbPj0iVk=</t>
   </si>
   <si>
-    <t>certificate_Скрипник_Александр_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/151C02okkrodek9XkNHwwL64-Lzsb2A4K/view</t>
   </si>
   <si>
     <t>Солонский Александр</t>
@@ -328,7 +328,7 @@
     <t>HJl2ppwA2A8OAdeoTUQgSeFpehYnbukxEkKsCk8a9B4cA67t4VuZQFywBceNl4+PyteA/KbcDlSe0tpcE0uy6KE=</t>
   </si>
   <si>
-    <t>certificate_Солонский_Александр_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1o8xLi-IHx4gfV0gb_0BtDtoGh7LtzNBR/view</t>
   </si>
   <si>
     <t>31.10.2016</t>
@@ -346,7 +346,7 @@
     <t>HNTazPdprjLP4Yf9ZgRIBFtjR6r25k2krvvvcDmOBhT6JfM8SxjU+De2Q5fzGm4VHpNMegOp06EnNohbpzpEMI4=</t>
   </si>
   <si>
-    <t>certificate_Anton_Zaporozhchenko_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/171HoquIjru4R_MMpzEry4G84W93iYfu0/view</t>
   </si>
   <si>
     <t>Oleksiy Ponomorev</t>
@@ -361,7 +361,7 @@
     <t>HJvFHdX5AJ/12PGL/ZqPsFvR5l1juzABjhdh9F/yKmyGNvsaHRsfmbR3HN3J1aLMHgGgTWiTuTKqMogk34LhS8g=</t>
   </si>
   <si>
-    <t>certificate_Oleksiy_Ponomorev_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1B4ym0awuGNI8pvWsBnktfyfbH-2WMDOs/view</t>
   </si>
   <si>
     <t>Pavel Brilliant</t>
@@ -376,7 +376,7 @@
     <t>G0QqHpt8SIjtEhZqu8ZwIdhaXdZLvLGNQMQTrINPsoNmdYf0Yp9854j+mcSOrLJh/dpq6aGZergC2+OcIJmIy5I=</t>
   </si>
   <si>
-    <t>certificate_Pavel_Brilliant_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1mQHe9fr1pAB162Y6DKpuoDRu20USBuia/view</t>
   </si>
   <si>
     <t>Volodymyr Kavetskyy</t>
@@ -391,7 +391,7 @@
     <t>HNthdNWPwGmVn+cxNWfoRfScs/fEnlCP9frX7t9Nc9waZeEkM3q1HPejLpswg7Zgr9y6nAgNqt4tQ5FnVGqczlc=</t>
   </si>
   <si>
-    <t>certificate_Volodymyr_Kavetskyy_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1pf2xfHz4QrHUfwdhOWh3HtkFWvLC6MCA/view</t>
   </si>
   <si>
     <t>Vladyslav Minakov</t>
@@ -406,7 +406,7 @@
     <t>G8QdtgHByifGkRpvkwoyqyHYBnvngvqGpsE0+OYg0l4/alH5hKrukluT0vymRI89FuPQaP5NZXhJw5qBqr/o2SQ=</t>
   </si>
   <si>
-    <t>certificate_Vladyslav_Minakov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1Sn9nXT9Fg-6kcdUTNymxwTxsf20gVtrG/view</t>
   </si>
   <si>
     <t>03.03.2017</t>
@@ -424,7 +424,7 @@
     <t>HA2ozpf6FmCR9/D/F1XgLiiwPlUjJLoag15bW5+L4fQHD0Fzs7c7/2KGC/bsQG8Qb9PP7XBe0ZLiDxxYN1sfvlc=</t>
   </si>
   <si>
-    <t>certificate_Yevheniia_Shchypeleva_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/19FD-029XSzp-hi7KhQ-AUDLjAIUUZ7CK/view</t>
   </si>
   <si>
     <t>Kolhatin Andrii</t>
@@ -439,7 +439,7 @@
     <t>HOcOQLZi/0Hj7wI2HfEnZo9/I0BIcJlvSIj0kM1p52IeZu906yz7HH82BuKoZn4vsU1NaeozhmLhrvaLuFl4axo=</t>
   </si>
   <si>
-    <t>certificate_Kolhatin_Andrii_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1fyOMT82rH5OEJhQA8RkME5jW_YXeZD0l/view</t>
   </si>
   <si>
     <t>Heorhii Kholodov</t>
@@ -454,7 +454,7 @@
     <t>G9GctEnd76pKgGDyI7+aE9V09Cbs9aumDPiqIQigvacdBmKIzpoQDCwHI7E+a/k9BOzv+g7d0xz+Gge0BLfJFfQ=</t>
   </si>
   <si>
-    <t>certificate_Heorhii_Kholodov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1d2uLNmRmxAUv8Ifvn89kCQZ1AsiBdBlV/view</t>
   </si>
   <si>
     <t>30.05.2018</t>
@@ -475,7 +475,7 @@
     <t>G+TKDQRHr+0M88vwYCpAR1HxlsZ9Z7wGKXvhaOHBU8VVVsZ6D827dqlCB+/VqOuSoiNUl2Q4njEuMlyVU8acWg0=</t>
   </si>
   <si>
-    <t>certificate_Aleksandr_Gnatyuk_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1LB_L4BZamLcp7AR1XoatjxLP0vVjCpx3/view</t>
   </si>
   <si>
     <t>Aleksandr Kurbatov</t>
@@ -490,7 +490,7 @@
     <t>HEGH5/OOhT4reguIiiTH6APFTbnlV5C1KUyZ1pDo2cj6OGuhq/LbQm/JPTRM/O7tZRuIRfzN9JFsrrjCWCFPlk4=</t>
   </si>
   <si>
-    <t>certificate_Aleksandr_Kurbatov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1snnHBWIknbRNiX0NedAZf3NtIRZNEJ-0/view</t>
   </si>
   <si>
     <t>Aleksandr Ivanov</t>
@@ -505,7 +505,7 @@
     <t>G3ZO9bxTgtB/7Fa9EI72atZVXvh2Ad/AFoyzzevZ8ZobO83vZr+y2kqGwnGR6W3RrWH6kTuo4FsGrD74ILRPfEY=</t>
   </si>
   <si>
-    <t>certificate_Aleksandr_Ivanov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/17mOMlQa1YhVjF_9FOaFabKNCB3ND3FQh/view</t>
   </si>
   <si>
     <t>Artyom Ahmetzyanov</t>
@@ -520,7 +520,7 @@
     <t>G6PuaRb177RpKrDmAjukXeT/Pov30l8TdCMgBJErT1YwH6DqSeI9ff2Z+uuJmeqveGXDYUhbYEhDxKg1jEaOK3E=</t>
   </si>
   <si>
-    <t>certificate_Artyom_Ahmetzyanov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/10ikHwrdBL6YjJRXXuqQ7kx-1p4kfuKs0/view</t>
   </si>
   <si>
     <t>Oleksii Khramov</t>
@@ -535,7 +535,7 @@
     <t>HBlAzPzVISCrhkXzo8GZ6W8Z84V6yqNwfy72EfWfgfhWCfoC3kzzdLh2hOyRRt8A/hleQIggp11lEkfjiBwU3FI=</t>
   </si>
   <si>
-    <t>certificate_Oleksii_Khramov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1TY0el-qpdd3EwZtfR2vdDMMp5P4-EfD2/view</t>
   </si>
   <si>
     <t>Nodar Alyoshin</t>
@@ -550,7 +550,7 @@
     <t>HAt2BcTILIRTPMZAwC+3r/wauy6mFamx0lLEvPl8T8u8X9L6TNJ2cd8B6X1E3f2E4izbyj19WA5Tr9VyW1AY1Qg=</t>
   </si>
   <si>
-    <t>certificate_Nodar_Alyoshin_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1FgquFxcBloQjUDkpBs_b69YTHR2ZqB87/view</t>
   </si>
   <si>
     <t>Marina Osadchuk</t>
@@ -565,7 +565,7 @@
     <t>G+SXoVDF+C1xZEypC8G1DkMNZU2K/YTniKoPmEOKvao7SAs1KY2p8RFoJlol9Hi5x+ZnLMocF64cXyB82fj4/co=</t>
   </si>
   <si>
-    <t>certificate_Marina_Osadchuk_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1rj5dK9gBRTFO__hNdfiUVQjuWQsBXc-h/view</t>
   </si>
   <si>
     <t>Konstantin Nechvolod</t>
@@ -580,7 +580,7 @@
     <t>HONq+40rWWcZg2ep51dVOeDlcPxRzZyoFaRcEx/kXFVcKkNrgAJWpl5iTfkoY7ClsA9dM+gU0ZZIXMolgSNmuIE=</t>
   </si>
   <si>
-    <t>certificate_Konstantin_Nechvolod_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1ERjLfWfliahHfDQz5DuanaYqSSRfF5rK/view</t>
   </si>
   <si>
     <t>Ilya Svetaylo</t>
@@ -595,7 +595,7 @@
     <t>HKkfJL99tKlg2eavVbzwdMxgOf61qj23+C38oRfT9S7yAurKw4uk38Arvj54gJ4diOc7XAAJJWI5WZpjkH+GVD4=</t>
   </si>
   <si>
-    <t>certificate_Ilya_Svetaylo_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1FtXae174jIJtBO_SrHZAM3wjIBDULjGP/view</t>
   </si>
   <si>
     <t>Dmytro Mandych</t>
@@ -610,7 +610,7 @@
     <t>GxJO7BiH7QSDOkaVyvoSs5I1l55gYnvxDt/EcTkBYowbQfUWr79pfg8SvoSGPtFFIAT16R5D3C2UWedyHqjSaq8=</t>
   </si>
   <si>
-    <t>certificate_Dmytro_Mandych_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1aOdfCvhxk_GkRDqQxoPGw2erGRgZ73X1/view</t>
   </si>
   <si>
     <t>26.05.2020</t>
@@ -631,7 +631,7 @@
     <t>HBzaIo/6pGkl+lxuK93TpLDR3J0fQnJuLF/UvSWu/DnCBGypnDxHHN+9YQPv6mCzEqy4c4ztULeBbX6umqneJbM=</t>
   </si>
   <si>
-    <t>certificate_Petr_Murzin_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1CeJnGVYu8FcIQ79Z-m9fldwUYFsXUJ6b/view</t>
   </si>
   <si>
     <t>28.05.2020</t>
@@ -649,7 +649,7 @@
     <t>HJg/1FFp+OhLbPPswjILag3FY2WMU4+XcI04Ns6LB9wmLexAfWDQnRgiXTtjkmQihRemlxaeqR6ftVepPZNrHBo=</t>
   </si>
   <si>
-    <t>certificate_Lovkin_Ivan_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1gkQ_FexA2nEy423To0DiDKIgnMzlxwn6/view</t>
   </si>
   <si>
     <t>30.05.2020</t>
@@ -667,7 +667,7 @@
     <t>HJncl4kaqw9zTObNyjKooaqcPCdEuHz5xHFvcd3MX5F8HVTSPlpFPcHe/I4J51+VrDAssyv3ithaKinCMpRryqA=</t>
   </si>
   <si>
-    <t>certificate_Nikita_Moskovkin_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1B0s8qbfjRTRziDEY223sdar5TrZ_cPnN/view</t>
   </si>
   <si>
     <t>03.06.2020</t>
@@ -685,7 +685,7 @@
     <t>Gzw/HIBgJ7KVFS7QmDgYWxq8XjKW4lAILc3sROoFzfxqWvK4tYRyGDb0ZvJKQe3xHaFC2CUeutLZSOTbfTa0QV0=</t>
   </si>
   <si>
-    <t>certificate_Valeriy_Gello_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1QVqrxbfAu2ZzG1arVdcCRvpou5O-dlCH/view</t>
   </si>
   <si>
     <t>21.08.2020</t>
@@ -703,7 +703,7 @@
     <t>HP41UyoLCOMLuOEIo42MuFafQWcp0t4i6LBAgNz75cNPYOBdXopZM+It2/Be2dr0ienxZVjSb3zJztSjlaD54l0=</t>
   </si>
   <si>
-    <t>certificate_Elizabeth_Gurieva_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1ZNXNNDuMq5S4WT-9rfZFU7tvavxGcahK/view</t>
   </si>
   <si>
     <t>15.09.2020</t>
@@ -721,7 +721,7 @@
     <t>HCzXH2Zbj4gbKDjETOQGCWS+XxeEZZMPOew3MUhUr0HhWixJ7eLggTl7cydDoD6sMmgIYDMN5sRHQ+XJ/Fvvb3Q=</t>
   </si>
   <si>
-    <t>certificate_Alexander_Zhovnuvaty_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1vaj0GQV6wKkBwRXRZbGnLtnn_YrT1O8v/view</t>
   </si>
   <si>
     <t>Nikolay Scherbakov</t>
@@ -736,7 +736,7 @@
     <t>HJJvBuSIMkoiAO+sC8QBznqFcgY8LSD1Gw6CvtwJSVJLYoihwr5NrQvIzV7l2SoU5cbCU+FRL/3euoLPhxfQyYM=</t>
   </si>
   <si>
-    <t>certificate_Nikolay_Scherbakov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/14nnUzKWQVeXgdJTK_F2ynBxFWahSA4Qg/view</t>
   </si>
   <si>
     <t>16.09.2020</t>
@@ -754,7 +754,7 @@
     <t>G4fHhUf678fe0keVwns3h0B7eDLW0jQOMkxJVRg9DwgKNOIjAgksa+fZ5mJ9Ojst1bHp2zGQfgVdtVILW+ZLpzY=</t>
   </si>
   <si>
-    <t>certificate_Anonymous_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/17KlJJSdt4WdpVK4WvalLDjUx3BaM1zEA/view</t>
   </si>
   <si>
     <t>17.09.2020</t>
@@ -772,7 +772,7 @@
     <t>HJvnMx8PPHp3/yBmcUPMH2FdjkOgbClzrn20BArlYjAnHxJJGArQJBD8smNoDbg1RsQNwFIkn+lLuOShvvcLCPY=</t>
   </si>
   <si>
-    <t>certificate_Aleksandr_Khomutov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1r5CZmD2VcuIsSLJqBl0pyKKAT2zPOnrl/view</t>
   </si>
   <si>
     <t>12.29.2021</t>
@@ -793,7 +793,7 @@
     <t>G3gYwhzI5+ZXB2kDCeqmw7ZIyAfM2VyNCo7rqfK6oErwXzOgVWTXTB2Y0nQTEsPVbu21i0aXTcjj1/cRs4q1Eh8=</t>
   </si>
   <si>
-    <t>certificate_Tetiana_Diachuk_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1-SMoX-EMMNtwbcEiKIY3QdjrEHX_3blE/view</t>
   </si>
   <si>
     <t>Yatskiv Vasyl</t>
@@ -808,7 +808,7 @@
     <t>HK7waE27kA6KJwApBM+T4LAk4aZqaE9IPDkBCxSy2kIEIufgsqcxvQ2rz19wEhtVeFadLyIdaeqHRdUIesIFeEY=</t>
   </si>
   <si>
-    <t>certificate_Yatskiv_Vasyl_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/10L1mno0hdZSlY3mp5M9ggKfImQbMX5b-/view</t>
   </si>
   <si>
     <t>24.05.2022</t>
@@ -826,7 +826,7 @@
     <t>HA5BwNFM/ySsemkCY6OpyYzGN2ynKMEaM8GLSihU2F8fIafDwOkoIh2PLwj1IdJ/pBYdBTic+Uho+017ECKjRNw=</t>
   </si>
   <si>
-    <t>certificate_Viktoriia_Kovalenko_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/11LC8uamJOa4HPIXAALboPtclhGduK0cu/view</t>
   </si>
   <si>
     <t>Artem Lytvynov</t>
@@ -841,7 +841,7 @@
     <t>Gyyl8SW1Vhxv2Y9izEr5P1xTWFuhrsh50Oxsq0ivOCIGYnrgsSq0dVAL7d/fHlQr4HKC5tRuFWRMg3E275kdLJs=</t>
   </si>
   <si>
-    <t>certificate_Artem_Lytvynov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1TfSgZrvfCTnKVfjpqX_sicX6OEQo-JZm/view</t>
   </si>
   <si>
     <t>Taras Horun</t>
@@ -856,7 +856,7 @@
     <t>HMm+QmgYSQqzfj+FdgRl1rWBCdL1S4zMjHo4rOlH25QqahXol4u5iYWlYHpMzEhlIt7GEVY6GQdrSoKBmssw+wE=</t>
   </si>
   <si>
-    <t>certificate_Taras_Horun_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1Yk5Ua8AHrOzAW-IEFp91vvo96m9atSht/view</t>
   </si>
   <si>
     <t>Anastasiia Slota</t>
@@ -871,7 +871,7 @@
     <t>HHSTW6baeeBbUdAqBUVAabWN7FyZcmoGl0a2yh2qMvM/NuSSlL5WIC4i/X4xl4ENs/MIKGxn/Yx4AQEZ3Xlfo/I=</t>
   </si>
   <si>
-    <t>certificate_Anastasiia_Slota_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1ccl1ojV7cJqlSm0tfLlfQjB7YYbW13U2/view</t>
   </si>
   <si>
     <t>Yuriy Melnychuk</t>
@@ -886,7 +886,7 @@
     <t>HLFj51cOIDt1qrqje2PXKxrtUxp1hjlrNJxyE2uD8TbiO2UKvbAI+WmR/rmJ3zP1nURKyFD3zP7orsfABAqigkg=</t>
   </si>
   <si>
-    <t>certificate_Yuriy_Melnychuk_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1Zyj_8jTpwmZDR3Ziq5I7K0sMtKzaNwzb/view</t>
   </si>
   <si>
     <t>Vladyslav Mazur</t>
@@ -901,7 +901,7 @@
     <t>HLRD02/6NJ7khwmd96Pm2n54FdjUOODqTq0B65DPCuq8DMRfhgsgzJhWRLUNGmka6qsOAlRYHVYcaFdURPX1T8I=</t>
   </si>
   <si>
-    <t>certificate_Vladyslav_Mazur_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1GDK3AFkFCTPOhHgHk3zBVNe6tX0OrNbU/view</t>
   </si>
   <si>
     <t>Hanna Zhurba</t>
@@ -916,7 +916,7 @@
     <t>G23T8nDlJs73D0lrECwkUe+mXYAtGdG9qjpSpWrU32pvXnfTe3DSqjCTi6rJFVs1Yzi2Fv3xylxp5MMR8p8VeRw=</t>
   </si>
   <si>
-    <t>certificate_Hanna_Zhurba_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1LG5dI_c4lGdx0g-N-E2xlZNflFVcGJB5/view</t>
   </si>
   <si>
     <t>Viktoriia Holoshchapova</t>
@@ -931,7 +931,10 @@
     <t>HNXgySG2kQ3jao+mFMaN3wfZFjEh5tNOLS3typW1XLu/AWlnZ9Wp8fZzONuZuA7Ld2EjAXGRflxYjsG/zZvNK1Y=</t>
   </si>
   <si>
-    <t>certificate_Viktoriia_Holoshchapova_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1WDfkJtWwN_7Eykowqn8g9kdv4c7k9i3d/view</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1VP-RZqDW14mfpj_KCvlLK1-g2-YAuDec/view</t>
   </si>
   <si>
     <t>Nikita Liashko</t>
@@ -946,7 +949,7 @@
     <t>HOt76U1Fm6QnHoInt0Smt+gAS3rWPhQyfPREvrRvrghaKyti2vcVHkLzN6+M0BSZWjdpmAEmApjrFE22eEaMtqg=</t>
   </si>
   <si>
-    <t>certificate_Nikita_Liashko_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1ClpQ380HsP3MS7usw0nzrDNHYj47DxNG/view</t>
   </si>
   <si>
     <t>27.05.2022</t>
@@ -964,7 +967,7 @@
     <t>HLH7WlOVLpwlLCX6S4IVdvTOunTc3QM9kpmouZBN7E+Lcd9pgsIPENfPEXdPoEc8HS/RGRqYc2669yxmo7TTYJI=</t>
   </si>
   <si>
-    <t>certificate_Oleksandr_Ishchuk_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1ykklygjmnrlmN1zdXNOBRgNAvzBf4AxN/view</t>
   </si>
   <si>
     <t>30.05.2022</t>
@@ -982,7 +985,7 @@
     <t>G5FFAmf/zMSc5uhA4w2of3MlPRCOl/nrSQ+EHORntQdSYge5OoFzcoywcRu+c8Al2Wn0vDT2gplOysnc9bkVKuU=</t>
   </si>
   <si>
-    <t>certificate_Sofiia_Zharkikh_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1dXF2b_CFYIEYDJzlj0JOjSaark_d_PEN/view</t>
   </si>
   <si>
     <t>Ruslan Ovsiienko</t>
@@ -997,7 +1000,7 @@
     <t>G3EE53pUm5VlTsbXpOwdRM63L+AGzsNrlmlAgBysqeKrQYUARmf1tqGI0uNbrYxulKqr9rUu9h6dgFSgLPwOlGo=</t>
   </si>
   <si>
-    <t>certificate_Ruslan_Ovsiienko_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1xxZab2PCK9hC-7J17Kb66qj0M6npYIRx/view</t>
   </si>
   <si>
     <t>31.05.2022</t>
@@ -1015,7 +1018,7 @@
     <t>HPxkFc6eqX1zkacNhXG+sBNXjVxyuH1KHnrh6B9b6e9zKf6E3ZsKgi7KviRGqMsROOkCltpUiNYA5H0saLu0V90=</t>
   </si>
   <si>
-    <t>certificate_Andrii_Kolhatin_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/171DkZ1tiXHoAUODWa2aGrDI5X307w6j0/view</t>
   </si>
   <si>
     <t>02.06.2022</t>
@@ -1033,7 +1036,7 @@
     <t>HKh9/uLqPvIlWlda72xmPBh4gWJPa1GmeUiFqmMUsnO2QBuonHk6hSItvca+oWB7KVakP8zuuiZy5E/0gh/gju8=</t>
   </si>
   <si>
-    <t>certificate_Volodymyr_Beimuk_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1ijEZMvPM3mLuQcb0a9DycWTOTVnwSBaS/view</t>
   </si>
   <si>
     <t>03.06.2022</t>
@@ -1051,7 +1054,7 @@
     <t>HNdZVHjhVExW+1Z4mN+Te9JfpSvd+YECTCgTdd9IJBnwfWKI4PH8xfVPvJr/RXDfqT+IXb/PUqhIJIfPeJabSSw=</t>
   </si>
   <si>
-    <t>certificate_Nazarii_Savorona_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1k2-p1WEYh08bNYBC61YD-g9cjGjXvPE7/view</t>
   </si>
   <si>
     <t>Anton Balykov</t>
@@ -1066,7 +1069,7 @@
     <t>HAcsbhV60MNVfxYYDPk95TsJ8K0vzClCraIHX3jcMxTUYWejpT1skkLDABMaWybvl4vDwSwhutHvP3VeuSN3hqQ=</t>
   </si>
   <si>
-    <t>certificate_Anton_Balykov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/15bpW11pqu9Gc4OdKxn1T9tGNCbGoxNmw/view</t>
   </si>
   <si>
     <t>06.06.2022</t>
@@ -1084,7 +1087,7 @@
     <t>G1SiRU5KQYfkC7uOSmRY/P2fj1w6YEu683um5h9a6ws8dlGMOSqTHYb8K/dSVioO+bMlb07pm5VcF6kewoJVWDQ=</t>
   </si>
   <si>
-    <t>certificate_Rodion_Nazarov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1sAClZogVz2jKXtG2YDHJ-IkoFjEDriRD/view</t>
   </si>
   <si>
     <t>Denis Riabtsev</t>
@@ -1099,7 +1102,7 @@
     <t>HFM+8AQaBKBacM/WH/81H8G44v3HvjExwoIa9nVWlJIta0EKSgLhtrtX6rhmpZuBXghHEk4mVxG+JFOMMQJ6+Cg=</t>
   </si>
   <si>
-    <t>certificate_Denis_Riabtsev_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1l5W4vY8nvFrLA3ziBPhdbhKRnQfXZAts/view</t>
   </si>
   <si>
     <t>10.08.2022</t>
@@ -1117,7 +1120,7 @@
     <t>HFa8giAwmh7H5tdphmNqPT2w8NyaSL0zoQtw8vhcOO24OJF8JiXHbFSXbqsuWnvYikzoLh9en0UUOiDdQ/qu9iM=</t>
   </si>
   <si>
-    <t>certificate_Ahadzhan_Piloian_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1vtYhJLBUaDUo1EcSWNbBKwVNJRSK0Un9/view</t>
   </si>
   <si>
     <t>16.08.2022</t>
@@ -1135,7 +1138,7 @@
     <t>HFDQ9yfu6U/EX1zGYWGMzuZllAhZ0Raovu7AG+Imc26Qa764AnS95/dSLQ7UQt9Go+rOAxw7mjemhwWS7bIocD8=</t>
   </si>
   <si>
-    <t>certificate_Andrii_Tsemko_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/15pKetGDmYgG84KN1SKFGRGxmow7QLlSx/view</t>
   </si>
   <si>
     <t>Oleg Chaika</t>
@@ -1150,7 +1153,7 @@
     <t>HGl/gXuPtt8M/8bCdJUa4gMn1i0me6N1NxOC/kl1Kbk6C7d/5u4zhbOjiYqYU38DGRQSiXH25MVys1FzzN3uYAQ=</t>
   </si>
   <si>
-    <t>certificate_Oleg_Chaika_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1M6mGUQ-FJOZ-vX9BxC8u1kEmpPGPlh6d/view</t>
   </si>
   <si>
     <t>Yehor Podporinov</t>
@@ -1165,7 +1168,7 @@
     <t>G2xO7B4Q+hdYRxBzyQaDhdsQu08oTGo4BF52Bl9If0c4DJKDCtwS9qoZx5Lj/2WEX02RiGVb6G02slDylbdqLAo=</t>
   </si>
   <si>
-    <t>certificate_Yehor_Podporinov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1wEN229hiH-jZ4o5y4aIpyhnZl_nu3XrJ/view</t>
   </si>
   <si>
     <t>Artem Litkevych</t>
@@ -1180,7 +1183,7 @@
     <t>HM6uF51YbAt3DbFxvVNTpeS9X1oDpHw0zFnNxLs999PuJNc1azg1gITStdzGKi8OvKjdT95PGN9f/sRqjNlY+2o=</t>
   </si>
   <si>
-    <t>certificate_Artem_Litkevych_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1NyxEt7-LRPN5TleCeayb9DdKjO5vn-Gt/view</t>
   </si>
   <si>
     <t>17.08.2022</t>
@@ -1198,7 +1201,7 @@
     <t>HOknl3bfOj6VWiF2cke75fBKUEhoJiAdgJIjzXMYR+mPe0Kx1XuF8nIHN+9jrnsbzNkPdUhb6jHrVKXTbhV8Q9w=</t>
   </si>
   <si>
-    <t>certificate_Vadim_Mokropulo_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/19-u8RS02tY_qjJDcHQDXvGPeMt8YNprQ/view</t>
   </si>
   <si>
     <t>Arsenii Trybukh</t>
@@ -1213,7 +1216,7 @@
     <t>HCM9Lxm2HfN4TKyTb1Hswsn5VJpsxgiJW5R+SepjJ0UeRlgsboEmN4/JokRrXfcmW+0+luqqgSqpIF/cWkAGIW0=</t>
   </si>
   <si>
-    <t>certificate_Arsenii_Trybukh_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1NmvZ2OYA8LdumUpH4j9qtkREpmootf-6/view</t>
   </si>
   <si>
     <t>18.08.2022</t>
@@ -1231,7 +1234,7 @@
     <t>G9Ch3H0JSIgK0D8+lUc+CVe5hh1/Qcz5M53LYvCPLGRtXm995jnkm8PhJ41ACFNTYNjNI1J86FZYJvp+vqILR7Y=</t>
   </si>
   <si>
-    <t>certificate_Khrystyna_Vysotska_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1f8zJGdzey9esgAdUPWtD6kQUfbVx__O-/view</t>
   </si>
   <si>
     <t>Mykhailo Shcholkin</t>
@@ -1246,7 +1249,7 @@
     <t>G21MICmkB2iY2fm+JV0nz2xQiarIBwVrE/zcp7NtMHxLGDcy+b6eWyg24mbfLxrYGHmHI7f2Ifh18c4LBUx6jd8=</t>
   </si>
   <si>
-    <t>certificate_Mykhailo_Shcholkin_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/12mJO_Dw8BIZV0CGf-aj5l2Y8kxaiFIou/view</t>
   </si>
   <si>
     <t>Sofiia Kireieva</t>
@@ -1261,7 +1264,7 @@
     <t>G69XJfmzHXDqV502Uhuy0UynJewLSZwOY17ZWoRWu+8fKZrLtItrl++E+920n1Az6u7sDFdBSFnUn8MMkLPmPrk=</t>
   </si>
   <si>
-    <t>certificate_Sofiia_Kireieva_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/18CvIeyXNErStjxQYS8XhnYZ_V0fSKP0q/view</t>
   </si>
   <si>
     <t>19.08.2022</t>
@@ -1279,7 +1282,7 @@
     <t>G2jP4FhVjFgaeIXACmuv4NrkTHbT4Pw2fsgVYqydLjTHTp2bFOhYi9tu99P7C6MSdtXuYAkVEk7jPkH9tPRKMPw=</t>
   </si>
   <si>
-    <t>certificate_Alena_Sporova_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/18mGx-WovdbPSZ22QCqMfgQ_mIMUrTLUK/view</t>
   </si>
   <si>
     <t>Nikita Masych</t>
@@ -1294,7 +1297,7 @@
     <t>HKdVLhA3gtAdaK2mauBkiowhnv2Evab2QPeel+p14+GqdfMA0rlCfRhIaFd8QEx1bwC62VO7N+ue3qNrejGq4vk=</t>
   </si>
   <si>
-    <t>certificate_Nikita_Masych_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/11bnDPBs0Z4Tj_2hpFCg_peAISN5R6gIw/view</t>
   </si>
   <si>
     <t>Mark Cherepovskyi</t>
@@ -1309,7 +1312,7 @@
     <t>G5B51sOpUq18kepe35rMw9WicCE1gp4icmIBoo3zjy+TD06p5inlInQt1WomW0tvEcye2foVrcdcBHrMqnC9pfo=</t>
   </si>
   <si>
-    <t>certificate_Mark_Cherepovskyi_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1NMsfhtCGGeNqpJ3Vf2HgCvk19dUtOhwl/view</t>
   </si>
   <si>
     <t>Viacheslav Horbanov</t>
@@ -1324,7 +1327,7 @@
     <t>HKpxDnYpWxDgjde7+Guu3BfglyLZHn8CSIxTn17IwxPuUfGHQDEVqrFM0MeyEBNAyZpkhKd/xI6fLRrcmAVWSDY=</t>
   </si>
   <si>
-    <t>certificate_Viacheslav_Horbanov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/17rAtt3AHNvQRSW_otXFUuED_C5oDmf9S/view</t>
   </si>
   <si>
     <t>22.08.2022</t>
@@ -1342,7 +1345,7 @@
     <t>HHQI2fVR8mK2cT2CKboOJcWp2QYPiQNiw9VPCxmosNu9XigtlaKhIcX6aeB7MeRagImuPo4PKFwP3lV41PaiRWM=</t>
   </si>
   <si>
-    <t>certificate_Oleksii_Stepaniuk_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1upztKMIWZAMZwzwAn_iKF2B8Rr0BC7YR/view</t>
   </si>
   <si>
     <t>Kyrylo Riabov</t>
@@ -1357,7 +1360,7 @@
     <t>HIYr22IoaZsHMt8mZYzRPItPizb8Cgz+tML67na5URpbDhO5czzxTUfp5REntqVtSPZLPmkfi+E9apG20T11FHM=</t>
   </si>
   <si>
-    <t>certificate_Kyrylo_Riabov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1iQqeJoHxEP0YA0U7RJpDnK5vZ5mW8RKx/view</t>
   </si>
   <si>
     <t>Oleksandr Kolesnyk</t>
@@ -1372,7 +1375,7 @@
     <t>G4lD8X41oRFy7CW2bmIknZKml/cSa36IX+BQ6GED5YydUXmGRs4WyhEEQrk67wJ4e1gzQZpb86PNONSIkqmbihc=</t>
   </si>
   <si>
-    <t>certificate_Oleksandr_Kolesnyk_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/13-JAJ-OjZ4zF9ZCcVufFE-oeoYARwZsy/view</t>
   </si>
   <si>
     <t>23.08.2022</t>
@@ -1390,7 +1393,7 @@
     <t>G8uS3y3E18j4FkL7WCCPvfCy3xbdDx3VvFRySq8LNas5LNV8IZyf7dLuyzgiueQoYXv/VtG+7WybSGkWdEvMw88=</t>
   </si>
   <si>
-    <t>certificate_Nikita_Chabaniuk_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1_nr-2NjQ9hDXjzNKowhjpTxCj3qgHz8c/view</t>
   </si>
   <si>
     <t>Amina Yambulatova</t>
@@ -1405,7 +1408,7 @@
     <t>G9g/25PmJHzczdwBSSy0Zypc9ZTw+/+YXHbvvw/DHm/9W+MgQkve2zHsaohfLfd1pXPsRJ+laHxZzzZgleauDAs=</t>
   </si>
   <si>
-    <t>certificate_Amina_Yambulatova_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1bScSOXDdNfMJxHR0zgGOUA7dGCyseMAw/view</t>
   </si>
   <si>
     <t>Yegor Chukanov</t>
@@ -1420,7 +1423,7 @@
     <t>HGwq4A8p8OWC5Gh+teNqjrwCzbrT0mWdm2OuDoYtB3s1HgthxjnTOjy9hI+EerJD42qx4NTjmyKAB9cpY84rOKg=</t>
   </si>
   <si>
-    <t>certificate_Yegor_Chukanov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1fMTVea461qNrzSGm-qGWFkRNfMM6iGqA/view</t>
   </si>
   <si>
     <t>24.08.2022</t>
@@ -1438,7 +1441,7 @@
     <t>G1juo7SBQZageFwRNPEys5X51AkNFvYuzGZjEuZEEItYJwfD03FjUeOtDPlRHnYj8rBLuAf/gCVBc2g1fV3w4wY=</t>
   </si>
   <si>
-    <t>certificate_Dmytro_Vynohradov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1pcMJ3o9R6KoVwjtb0mi4YiiDPEcFfWoI/view</t>
   </si>
   <si>
     <t>Mykhailo Sokolov</t>
@@ -1453,7 +1456,7 @@
     <t>HIqeKGpM6CeW69LC2KUeOJ9DRnIDBY+r995bjEVZo8pLDWXucjkEriUeL8WyPveeSxxPg7hM8PqDICAEPlVCouk=</t>
   </si>
   <si>
-    <t>certificate_Mykhailo_Sokolov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1VAL0MrEV46yshybWqnwVMSv0QFDsN8Js/view</t>
   </si>
   <si>
     <t>25.08.2022</t>
@@ -1471,7 +1474,7 @@
     <t>G8mavASwRAESd8slmxm1h9U4N6GoYmgCKDKXl8T/zpv6KTqrqhp1n8tXhH7flfqxI88ksENHVZ8D+dYALB3M5Xo=</t>
   </si>
   <si>
-    <t>certificate_Illia_Popov_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1zbXRc6VreZpRvoTuXAFHhk6A7ivLCjBe/view</t>
   </si>
   <si>
     <t>26.08.2022</t>
@@ -1489,7 +1492,7 @@
     <t>Gw56LuM5gYEPRCkhmZ6K29DG3idPfq6lawS2onGmpo38efTvJlIFfopETOm/W1WkS+UuYHQsremfscaqHR3acyY=</t>
   </si>
   <si>
-    <t>certificate_Mykola_Gora_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1iFipfjcgBdka6coxpE7L6OQ6Gra6gB8L/view</t>
   </si>
   <si>
     <t>Artem Levkin</t>
@@ -1504,7 +1507,7 @@
     <t>G8ah5f2UjwoYEixl7OZKZrVAizGnQBy+lwuL+ammNcBqEjR8riRwunMmhjuzXKnQ8orFQJXmZhMvaCtDzItFhnw=</t>
   </si>
   <si>
-    <t>certificate_Artem_Levkin_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1Oi13CqgC7cobG-poXCyQ9Ml_VaIyziRW/view</t>
   </si>
   <si>
     <t>29.08.2022</t>
@@ -1522,7 +1525,7 @@
     <t>G0ZjvUb5sgyD719aQ7ygiXigPsrGpMAmw0TdIjX2xBb4BuYLIXwlOY1LYnd5sdVo6jKKXK6g1s4UIJKuU8RPHew=</t>
   </si>
   <si>
-    <t>certificate_Natalya_Dolgova_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1MODb54QOY9wkT1MlOxHoNNqUnb67e-R-/view</t>
   </si>
   <si>
     <t>Artem Zubrych</t>
@@ -1537,7 +1540,7 @@
     <t>GzMrbbTOSSl0/ql8CiImmJSDgqgJUtSq87qEm3e4f1HUDlkuor0IcoFP2Jf9vSiQXbE3YJaOZ40DHqr8oSg+roc=</t>
   </si>
   <si>
-    <t>certificate_Artem_Zubrych_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/13Dv6C66JsAvW76y5AegaNsdLparwFuIY/view</t>
   </si>
   <si>
     <t>30.08.2022</t>
@@ -1555,7 +1558,7 @@
     <t>HIhvyjj7WGrwrUbsuWPUTAKqKtxfC9u3gJ1V8w+AsfkMDrZmymnpA/ScCurlcuX7M6q7OXFso7OfbFtzTlNkx0E=</t>
   </si>
   <si>
-    <t>certificate_Valentyna_Lytvynova_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1-WUf_Jobf4VArFm8VEO1WYjef5YKJtpz/view</t>
   </si>
   <si>
     <t>Eugene Petrikeev</t>
@@ -1570,7 +1573,7 @@
     <t>G2ZueU8SyB00Pru2Gbk4Y4zUXtkuEm3BwdBArAtr5mwqa3CSk8hS/tw/n3taWXsYOLN2wbMWQWcfsBiEFlUB3+Q=</t>
   </si>
   <si>
-    <t>certificate_Eugene_Petrikeev_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1y8vgpGbLCd4ygBhGfs-BdcGPCPM7e5ol/view</t>
   </si>
   <si>
     <t>Yurii Poberezhnyi</t>
@@ -1585,7 +1588,7 @@
     <t>G7odIa2nR2CTXihZ272zal5AhXr13DqLqqyxkYgyuEN7cLxIlWKECJnfXCeXzPqGH8fBfl9v7DunBuqlObCkULE=</t>
   </si>
   <si>
-    <t>certificate_Yurii_Poberezhnyi_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/13owzToVXMW-D4sr706sfC3WbeSfs1dm4/view</t>
   </si>
   <si>
     <t>07.09.2022</t>
@@ -1603,7 +1606,7 @@
     <t>HAFRgVQFeujXBXYVTCe8VE2auw6Uz+L7Lzq6SSmMkvoEYyvkGFCp6L0hO5+CtccnYIEPL5r5hiDHuG6deADYunw=</t>
   </si>
   <si>
-    <t>certificate_Alina_Telnova_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1_3nb1PAXgUPHALmaPXZGiITZBF1bi93a/view</t>
   </si>
   <si>
     <t>07.12.2022</t>
@@ -1624,7 +1627,7 @@
     <t>Gxb5qLCO2gOVk0XmAl5V0xEK4mWcrjqA5qw51GpsOz7mIajkq6+QkZj9qyqPbzcd2vRlji2whyQPpa58B92Jpw4=</t>
   </si>
   <si>
-    <t>certificate_Oleksandra_Ivanova_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1RwFFLutPf7MS5BUl5bg_lZnb2PKu3Voj/view</t>
   </si>
   <si>
     <t>08.12.2022</t>
@@ -1642,7 +1645,7 @@
     <t>HDb3/S0qJ/hv7vYMP1ZqYnk4Y8RcwlpISSEsOQrArUPGQj4lAL1fzpn7iRYLH23LEYv1ECvia7I/aGki2RCqb/s=</t>
   </si>
   <si>
-    <t>certificate_Ilona_Shevchenko_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1wIJgfjKmEmEbDPiAD3I3M7V1M_3dY47I/view</t>
   </si>
   <si>
     <t>Ievgeniia Bondar</t>
@@ -1657,7 +1660,7 @@
     <t>HIgwLjNpC9EMttrwVCHCqYNaw9oP6JDSNC3WNNknWncLPhG4ednynhWTcdaeAX+FwguxVwPvX9m7LvvlPFKLdrQ=</t>
   </si>
   <si>
-    <t>certificate_Ievgeniia_Bondar_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1aJAputdo62hrvrHWqsqQQ72U0zr9q9wz/view</t>
   </si>
   <si>
     <t>Sofia Golets</t>
@@ -1672,7 +1675,7 @@
     <t>HBabTC2ygOQ+iqxIRo7A4uu6gllcQml5FLggMVySfR6Db60y77BToxgXwXmdwrHtoN1Gua5C8I7MgdjeDLZ8JCo=</t>
   </si>
   <si>
-    <t>certificate_Sofia_Golets_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1L9C0OIiKRM1iU9FCn57hsUlyxGwsmfkM/view</t>
   </si>
   <si>
     <t>Mykyta Tsyvinskyi</t>
@@ -1687,7 +1690,7 @@
     <t>HPq9RQ1vlbJ4N83dgUwLLBJcN4AFaUJYC8F8BVzxUkYDR6OqA/YcNOeiukloL3UmZXPkluIN4lwoBhMr6vEj8KA=</t>
   </si>
   <si>
-    <t>certificate_Mykyta_Tsyvinskyi_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1xfil2bz5LPldBY--aAdQvyDpsss0CHNz/view</t>
   </si>
   <si>
     <t>Cryptography and information security theory</t>
@@ -1702,6 +1705,9 @@
     <t>G+LRDlMfhyvZO7qLoCtZi3Y4Q1yC/VmYJUOF79rRwGAGH93HyPOn0ZUp6fjZE87K+JkhhSiBVl2Pf+AGfNu10RA=</t>
   </si>
   <si>
+    <t>https://drive.google.com/file/d/1A5-xfWa0l4aHueUyg8UFsv7EFEE_XPS-/view</t>
+  </si>
+  <si>
     <t>09.12.2022</t>
   </si>
   <si>
@@ -1714,6 +1720,9 @@
     <t>G8FalVqgQocrfJLlZmP9e76Z9t26v1gwrDzzjckei89eQgv6utrC5/Tx62NoCPt1u4EWkCFyccyEuy8FOsOnjtM=</t>
   </si>
   <si>
+    <t>https://drive.google.com/file/d/1_zWg-rCl08UMxstB2z3rz4f-zl_3mYp9/view</t>
+  </si>
+  <si>
     <t>Kateryna Hordiienko</t>
   </si>
   <si>
@@ -1726,7 +1735,7 @@
     <t>G+YE6/0P9zPNxZ1YU3AR+TXthT9PlF8Gx3dM9k7Y2cNIIrTalRdUgSTwwSMu/mcimZUsZLZ5l2puCtwVP6ll5kI=</t>
   </si>
   <si>
-    <t>certificate_Kateryna_Hordiienko_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1XvSjTye5r2MvVX1NBBYIyTI3jFMXzIBu/view</t>
   </si>
   <si>
     <t>12.12.2022</t>
@@ -1741,6 +1750,9 @@
     <t>G11bw0NMOTyr+kZ3HiySXxlzt4gjcFWjXTypvr6Lhl5sbFSVpzIzmc9E4TVP/fDQXH5yEqb67EOF8dGgrWOyXOU=</t>
   </si>
   <si>
+    <t>https://drive.google.com/file/d/1I72Eozicc1xL9Y5sCJwxxjfmYVxcs7HU/view</t>
+  </si>
+  <si>
     <t>Yuliia Aritkulova</t>
   </si>
   <si>
@@ -1753,7 +1765,7 @@
     <t>HGoEk/y9kiwBSF9cMiOClOSNtviGjcJylz3TuZUULAVcC8Gx1XGbVYWpWMB4aLPfkZhN7OKce2kkKQ9ADcgzaHI=</t>
   </si>
   <si>
-    <t>certificate_Yuliia_Aritkulova_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1Jxt54lK7qfn3swmTW78tfF0azSbE6B-E/view</t>
   </si>
   <si>
     <t>Oleksandr Yevtushenko</t>
@@ -1768,7 +1780,7 @@
     <t>G9WI+TMiMLY1UW9rtOW0ycI21KtE3yOBTQ511sJbmfIXWvRQanASycY6fUpVGhO7iM8gyJxecc4xx2ytHX1VgzY=</t>
   </si>
   <si>
-    <t>certificate_Oleksandr_Yevtushenko_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1zDtxSunJrT77cm6IM6IY9mTY4mqeL_np/view</t>
   </si>
   <si>
     <t>Mariia Mahdalina</t>
@@ -1783,7 +1795,7 @@
     <t>HAxDgAqvSDtLYbdDhyc88l9igZ8/dmzp3+4TAVQXHMelL+qELJVHvRnOAobpaXU7p8Rj9a7taRtzW/nkCowSS5U=</t>
   </si>
   <si>
-    <t>certificate_Mariia_Mahdalina_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1SuncGKB7pEQHOf2s_qqYBfLNjupcIaw_/view</t>
   </si>
   <si>
     <t>766041da4e35a4d0486d</t>
@@ -1795,6 +1807,9 @@
     <t>G6T2wslW9Mlopb7SNt9oGcOSZmjSMvsByzfIQBZfwVweUZ7U2Mi5N0BkW7xhpRFkMMCWlY1kHu4VefyQzGyK5dA=</t>
   </si>
   <si>
+    <t>https://drive.google.com/file/d/1ATEuTKOXmHhIdtjgFN8iUX5fFdGo2Wfr/view</t>
+  </si>
+  <si>
     <t>13.12.2022</t>
   </si>
   <si>
@@ -1810,7 +1825,7 @@
     <t>HJVKQ2Uj9PkXKh4aB7EUy+qqEtzziBAX7CaNWYTiFDyXIQ5w6CG1bIat2vs1GsmBD+r6z55FbUFJFdXz57+QgUc=</t>
   </si>
   <si>
-    <t>certificate_Anastasia_Andreeva_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1lqwakseXObG2YQiGwS5h-GQI_nDbjzor/view</t>
   </si>
   <si>
     <t>Polina Reshetnikova</t>
@@ -1825,7 +1840,7 @@
     <t>G63Lq+BtAcEqpIZphPzrLfd1K4chy2llUoMMBLMQGk5gdyNM+62UvBxqqOxckVeN2RtGC1vCiL0NvWNvEPfV4YE=</t>
   </si>
   <si>
-    <t>certificate_Polina_Reshetnikova_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1i117YwnGjmsgELq5E7XDbQhuxDXicUJB/view</t>
   </si>
   <si>
     <t>93620030db08953cbf17</t>
@@ -1837,6 +1852,9 @@
     <t>HHbiD8H1z2fwCjgA0K/0GymJl4RcCi3wnehCfa72EOF+RwXPgmdTom5TH/IQ6e5AjmLndgB/4YfHFtdBTD1hpx0=</t>
   </si>
   <si>
+    <t>https://drive.google.com/file/d/1tTlWJe1RfLa3p4a1IxEBhPf7Fp0yzXaA/view</t>
+  </si>
+  <si>
     <t>b3240a1974bff838f353</t>
   </si>
   <si>
@@ -1846,6 +1864,9 @@
     <t>HE5sTfhDSPPfvHdDSYkSvX2ZkktsyYMaoVxamHtpKMWoUxr7olw6SaItyMSztkPit37aQqfQ+YAsvCfZ01AcAwc=</t>
   </si>
   <si>
+    <t>https://drive.google.com/file/d/1_c7JvqJa0gEW9ebJyTS3goD51HqYmEMH/view</t>
+  </si>
+  <si>
     <t>14.12.2022</t>
   </si>
   <si>
@@ -1858,6 +1879,9 @@
     <t>G6+s7V2DHLaRMUYNOIA8N40KmelApLWT3iXHGYHXv0ZJIGVzGNez6R9Ai+af6Go130PTYDBGSDSN/q4KZdDYaqI=</t>
   </si>
   <si>
+    <t>https://drive.google.com/file/d/1qsjfa4wL1t1quP9wJnR9cBbl7xkkw7sw/view</t>
+  </si>
+  <si>
     <t>Pasha Charovatiy</t>
   </si>
   <si>
@@ -1870,7 +1894,7 @@
     <t>G7RWOhYR3Pga7E8mj5Et4kkWc7KuUetPMGwNK9GBcXidXEmOn5A4bZr6u3pSr5OoaxZ8UjdHdb0bTK1X7lEavnk=</t>
   </si>
   <si>
-    <t>certificate_Pasha_Charovatiy_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1c17o-UNBE3C2Osr4odB0JBZRQmBdLVEG/view</t>
   </si>
   <si>
     <t>Dmytro Serhiienko</t>
@@ -1885,7 +1909,7 @@
     <t>G2X/6IWqMC2Ymk+rqd3pVM249KmwfExvjnsilLmKcIDST7fVzip5FqwERspfBc+vRT9X3TLONlOopGsxmrlg66Y=</t>
   </si>
   <si>
-    <t>certificate_Dmytro_Serhiienko_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1vNRTAtkFKZzILmmXVpV3QO-3VE-P-dGo/view</t>
   </si>
   <si>
     <t>Vladislav Dmitrenko</t>
@@ -1900,7 +1924,7 @@
     <t>HFVHGzz5fLLwIDpbXHtv3bag0i23gGXtR9qTV+i7/M17V/LEtIWkrIvmP+sVC0DQ2HxtNux5N00OioXu96ZQt+8=</t>
   </si>
   <si>
-    <t>certificate_Vladislav_Dmitrenko_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1uDrbsupU_qxrxoG3EqWtPGqh4wV0IzfA/view</t>
   </si>
   <si>
     <t>Marina Rindina</t>
@@ -1915,7 +1939,7 @@
     <t>HGAKfmnHj8txRq9vnJYL+4CzcrKQOcEeeUcwmL008Qw+BXNOZF20s86M17JhYF8d9ABQnHhRnj+X5d3DsBWt/74=</t>
   </si>
   <si>
-    <t>certificate_Marina_Rindina_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1oqZlbveMHgPlcfC9iWVuYzC5PSYCP8qG/view</t>
   </si>
   <si>
     <t>15.12.2022</t>
@@ -1933,7 +1957,7 @@
     <t>HL/mv02dnaeyvxsR9TyKJfqMl9lFEn1L8OidD6AzOq6SbieHRkQRPK29os5vKBwoJ5+Bf7RtfN9xUiVEOCASXj0=</t>
   </si>
   <si>
-    <t>certificate_Nazar_Franko_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1SlHKFR513B1XXyAwNg2rNpvmhHKKFQiv/view</t>
   </si>
   <si>
     <t>Olha Drahomeretska</t>
@@ -1948,7 +1972,7 @@
     <t>HErdMQ+2CPtlOJcP0I5vxghyuQmJVGZrrQr9SzMolPyHA1fUnzBjAbN7DzwkyP+y7M+dkiNCGOkNsY3YZaCO1XA=</t>
   </si>
   <si>
-    <t>certificate_Olha_Drahomeretska_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/11GQcoK_MALyH4TC6IpaHAlkbN7qEoChQ/view</t>
   </si>
   <si>
     <t>Maksym Cherniak</t>
@@ -1963,7 +1987,7 @@
     <t>HFsvImraI1pnG2rg4i0wdJncZx8WDDmyLmfp4YGsC/EJOrFIARj32EBYcrPX9GvGkI5YQdTVz4kCHGI7Y1+kc/s=</t>
   </si>
   <si>
-    <t>certificate_Maksym_Cherniak_QR_codecreate.svg</t>
+    <t>https://drive.google.com/file/d/1RiaqirxFepm7_yOvW1jzV-FlJT58zofz/view</t>
   </si>
   <si>
     <t>3bf214d846d708bfad51</t>
@@ -1973,6 +1997,9 @@
   </si>
   <si>
     <t>HDfq7iIvfl/KNv5Cs/GPeiZndLZYqskpWWIXt7VX3LunRfVInSqJiTeO33MHHKI8aX3Zz4VgDh7LV5fAg/zZPZk=</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1gXbm-vdryeb44xvOsLiA0RzMq6c7Cq14/view</t>
   </si>
 </sst>
 </file>
@@ -4103,7 +4130,7 @@
         <v>269</v>
       </c>
       <c r="J57" t="s">
-        <v>270</v>
+        <v>306</v>
       </c>
     </row>
     <row r="58">
@@ -4111,13 +4138,13 @@
         <v>265</v>
       </c>
       <c r="B58" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C58" t="s">
         <v>255</v>
       </c>
       <c r="D58" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E58" t="s">
         <v>14</v>
@@ -4126,30 +4153,30 @@
         <v>14</v>
       </c>
       <c r="G58" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H58" t="s">
         <v>14</v>
       </c>
       <c r="I58" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="J58" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B59" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C59" t="s">
         <v>255</v>
       </c>
       <c r="D59" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E59" t="s">
         <v>14</v>
@@ -4158,30 +4185,30 @@
         <v>14</v>
       </c>
       <c r="G59" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H59" t="s">
         <v>14</v>
       </c>
       <c r="I59" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="J59" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B60" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C60" t="s">
         <v>255</v>
       </c>
       <c r="D60" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E60" t="s">
         <v>14</v>
@@ -4190,30 +4217,30 @@
         <v>14</v>
       </c>
       <c r="G60" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H60" t="s">
         <v>14</v>
       </c>
       <c r="I60" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="J60" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B61" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C61" t="s">
         <v>255</v>
       </c>
       <c r="D61" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E61" t="s">
         <v>14</v>
@@ -4222,30 +4249,30 @@
         <v>14</v>
       </c>
       <c r="G61" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="H61" t="s">
         <v>14</v>
       </c>
       <c r="I61" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="J61" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B62" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C62" t="s">
         <v>255</v>
       </c>
       <c r="D62" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E62" t="s">
         <v>14</v>
@@ -4254,30 +4281,30 @@
         <v>14</v>
       </c>
       <c r="G62" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="H62" t="s">
         <v>14</v>
       </c>
       <c r="I62" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="J62" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B63" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C63" t="s">
         <v>255</v>
       </c>
       <c r="D63" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E63" t="s">
         <v>14</v>
@@ -4286,30 +4313,30 @@
         <v>14</v>
       </c>
       <c r="G63" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H63" t="s">
         <v>14</v>
       </c>
       <c r="I63" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="J63" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B64" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C64" t="s">
         <v>255</v>
       </c>
       <c r="D64" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E64" t="s">
         <v>14</v>
@@ -4318,30 +4345,30 @@
         <v>14</v>
       </c>
       <c r="G64" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="H64" t="s">
         <v>14</v>
       </c>
       <c r="I64" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="J64" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B65" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C65" t="s">
         <v>255</v>
       </c>
       <c r="D65" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E65" t="s">
         <v>14</v>
@@ -4350,30 +4377,30 @@
         <v>14</v>
       </c>
       <c r="G65" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="H65" t="s">
         <v>14</v>
       </c>
       <c r="I65" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="J65" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B66" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C66" t="s">
         <v>255</v>
       </c>
       <c r="D66" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E66" t="s">
         <v>14</v>
@@ -4382,30 +4409,30 @@
         <v>14</v>
       </c>
       <c r="G66" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H66" t="s">
         <v>14</v>
       </c>
       <c r="I66" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="J66" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B67" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C67" t="s">
         <v>255</v>
       </c>
       <c r="D67" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E67" t="s">
         <v>14</v>
@@ -4414,30 +4441,30 @@
         <v>14</v>
       </c>
       <c r="G67" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="H67" t="s">
         <v>14</v>
       </c>
       <c r="I67" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="J67" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B68" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C68" t="s">
         <v>255</v>
       </c>
       <c r="D68" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E68" t="s">
         <v>14</v>
@@ -4446,30 +4473,30 @@
         <v>14</v>
       </c>
       <c r="G68" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H68" t="s">
         <v>14</v>
       </c>
       <c r="I68" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="J68" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B69" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C69" t="s">
         <v>255</v>
       </c>
       <c r="D69" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E69" t="s">
         <v>14</v>
@@ -4478,30 +4505,30 @@
         <v>14</v>
       </c>
       <c r="G69" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="H69" t="s">
         <v>14</v>
       </c>
       <c r="I69" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="J69" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B70" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C70" t="s">
         <v>255</v>
       </c>
       <c r="D70" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E70" t="s">
         <v>14</v>
@@ -4510,30 +4537,30 @@
         <v>14</v>
       </c>
       <c r="G70" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H70" t="s">
         <v>14</v>
       </c>
       <c r="I70" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="J70" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B71" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C71" t="s">
         <v>255</v>
       </c>
       <c r="D71" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E71" t="s">
         <v>14</v>
@@ -4542,30 +4569,30 @@
         <v>14</v>
       </c>
       <c r="G71" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H71" t="s">
         <v>14</v>
       </c>
       <c r="I71" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="J71" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B72" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C72" t="s">
         <v>255</v>
       </c>
       <c r="D72" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E72" t="s">
         <v>14</v>
@@ -4574,30 +4601,30 @@
         <v>14</v>
       </c>
       <c r="G72" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H72" t="s">
         <v>14</v>
       </c>
       <c r="I72" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="J72" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B73" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C73" t="s">
         <v>255</v>
       </c>
       <c r="D73" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E73" t="s">
         <v>14</v>
@@ -4606,30 +4633,30 @@
         <v>14</v>
       </c>
       <c r="G73" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="H73" t="s">
         <v>14</v>
       </c>
       <c r="I73" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="J73" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B74" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C74" t="s">
         <v>255</v>
       </c>
       <c r="D74" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E74" t="s">
         <v>14</v>
@@ -4638,30 +4665,30 @@
         <v>14</v>
       </c>
       <c r="G74" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="H74" t="s">
         <v>14</v>
       </c>
       <c r="I74" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="J74" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B75" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C75" t="s">
         <v>255</v>
       </c>
       <c r="D75" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E75" t="s">
         <v>14</v>
@@ -4670,30 +4697,30 @@
         <v>14</v>
       </c>
       <c r="G75" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="H75" t="s">
         <v>14</v>
       </c>
       <c r="I75" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="J75" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B76" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C76" t="s">
         <v>255</v>
       </c>
       <c r="D76" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E76" t="s">
         <v>14</v>
@@ -4702,30 +4729,30 @@
         <v>14</v>
       </c>
       <c r="G76" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="H76" t="s">
         <v>14</v>
       </c>
       <c r="I76" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="J76" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B77" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C77" t="s">
         <v>255</v>
       </c>
       <c r="D77" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E77" t="s">
         <v>14</v>
@@ -4734,30 +4761,30 @@
         <v>14</v>
       </c>
       <c r="G77" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="H77" t="s">
         <v>14</v>
       </c>
       <c r="I77" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="J77" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B78" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C78" t="s">
         <v>255</v>
       </c>
       <c r="D78" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E78" t="s">
         <v>14</v>
@@ -4766,30 +4793,30 @@
         <v>14</v>
       </c>
       <c r="G78" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H78" t="s">
         <v>14</v>
       </c>
       <c r="I78" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="J78" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B79" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C79" t="s">
         <v>255</v>
       </c>
       <c r="D79" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E79" t="s">
         <v>14</v>
@@ -4798,30 +4825,30 @@
         <v>14</v>
       </c>
       <c r="G79" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H79" t="s">
         <v>14</v>
       </c>
       <c r="I79" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="J79" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B80" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C80" t="s">
         <v>255</v>
       </c>
       <c r="D80" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E80" t="s">
         <v>14</v>
@@ -4830,30 +4857,30 @@
         <v>14</v>
       </c>
       <c r="G80" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H80" t="s">
         <v>14</v>
       </c>
       <c r="I80" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="J80" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B81" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C81" t="s">
         <v>255</v>
       </c>
       <c r="D81" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E81" t="s">
         <v>14</v>
@@ -4862,30 +4889,30 @@
         <v>14</v>
       </c>
       <c r="G81" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H81" t="s">
         <v>14</v>
       </c>
       <c r="I81" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="J81" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B82" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C82" t="s">
         <v>255</v>
       </c>
       <c r="D82" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E82" t="s">
         <v>14</v>
@@ -4894,30 +4921,30 @@
         <v>14</v>
       </c>
       <c r="G82" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H82" t="s">
         <v>14</v>
       </c>
       <c r="I82" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="J82" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B83" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C83" t="s">
         <v>255</v>
       </c>
       <c r="D83" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E83" t="s">
         <v>14</v>
@@ -4926,30 +4953,30 @@
         <v>14</v>
       </c>
       <c r="G83" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="H83" t="s">
         <v>14</v>
       </c>
       <c r="I83" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="J83" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B84" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C84" t="s">
         <v>255</v>
       </c>
       <c r="D84" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E84" t="s">
         <v>14</v>
@@ -4958,30 +4985,30 @@
         <v>14</v>
       </c>
       <c r="G84" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H84" t="s">
         <v>14</v>
       </c>
       <c r="I84" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="J84" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B85" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C85" t="s">
         <v>255</v>
       </c>
       <c r="D85" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E85" t="s">
         <v>14</v>
@@ -4990,30 +5017,30 @@
         <v>14</v>
       </c>
       <c r="G85" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H85" t="s">
         <v>14</v>
       </c>
       <c r="I85" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="J85" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B86" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C86" t="s">
         <v>255</v>
       </c>
       <c r="D86" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="E86" t="s">
         <v>14</v>
@@ -5022,30 +5049,30 @@
         <v>14</v>
       </c>
       <c r="G86" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="H86" t="s">
         <v>14</v>
       </c>
       <c r="I86" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="J86" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B87" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C87" t="s">
         <v>255</v>
       </c>
       <c r="D87" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E87" t="s">
         <v>14</v>
@@ -5054,30 +5081,30 @@
         <v>14</v>
       </c>
       <c r="G87" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="H87" t="s">
         <v>14</v>
       </c>
       <c r="I87" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="J87" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B88" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C88" t="s">
         <v>255</v>
       </c>
       <c r="D88" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E88" t="s">
         <v>14</v>
@@ -5086,30 +5113,30 @@
         <v>14</v>
       </c>
       <c r="G88" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="H88" t="s">
         <v>14</v>
       </c>
       <c r="I88" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="J88" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B89" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C89" t="s">
         <v>255</v>
       </c>
       <c r="D89" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E89" t="s">
         <v>14</v>
@@ -5118,30 +5145,30 @@
         <v>14</v>
       </c>
       <c r="G89" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="H89" t="s">
         <v>14</v>
       </c>
       <c r="I89" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="J89" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B90" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C90" t="s">
         <v>255</v>
       </c>
       <c r="D90" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="E90" t="s">
         <v>14</v>
@@ -5150,30 +5177,30 @@
         <v>14</v>
       </c>
       <c r="G90" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="H90" t="s">
         <v>14</v>
       </c>
       <c r="I90" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="J90" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B91" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C91" t="s">
         <v>255</v>
       </c>
       <c r="D91" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E91" t="s">
         <v>14</v>
@@ -5182,30 +5209,30 @@
         <v>14</v>
       </c>
       <c r="G91" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="H91" t="s">
         <v>14</v>
       </c>
       <c r="I91" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="J91" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B92" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C92" t="s">
         <v>255</v>
       </c>
       <c r="D92" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E92" t="s">
         <v>14</v>
@@ -5214,30 +5241,30 @@
         <v>14</v>
       </c>
       <c r="G92" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="H92" t="s">
         <v>14</v>
       </c>
       <c r="I92" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="J92" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B93" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C93" t="s">
         <v>255</v>
       </c>
       <c r="D93" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E93" t="s">
         <v>14</v>
@@ -5246,30 +5273,30 @@
         <v>14</v>
       </c>
       <c r="G93" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="H93" t="s">
         <v>14</v>
       </c>
       <c r="I93" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="J93" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B94" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C94" t="s">
         <v>255</v>
       </c>
       <c r="D94" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="E94" t="s">
         <v>14</v>
@@ -5278,30 +5305,30 @@
         <v>14</v>
       </c>
       <c r="G94" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H94" t="s">
         <v>14</v>
       </c>
       <c r="I94" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="J94" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B95" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C95" t="s">
         <v>255</v>
       </c>
       <c r="D95" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E95" t="s">
         <v>14</v>
@@ -5310,30 +5337,30 @@
         <v>14</v>
       </c>
       <c r="G95" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="H95" t="s">
         <v>14</v>
       </c>
       <c r="I95" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="J95" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B96" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C96" t="s">
         <v>255</v>
       </c>
       <c r="D96" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E96" t="s">
         <v>14</v>
@@ -5342,30 +5369,30 @@
         <v>14</v>
       </c>
       <c r="G96" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="H96" t="s">
         <v>14</v>
       </c>
       <c r="I96" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="J96" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B97" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C97" t="s">
         <v>255</v>
       </c>
       <c r="D97" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E97" t="s">
         <v>14</v>
@@ -5374,30 +5401,30 @@
         <v>14</v>
       </c>
       <c r="G97" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="H97" t="s">
         <v>14</v>
       </c>
       <c r="I97" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="J97" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B98" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C98" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D98" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E98" t="s">
         <v>14</v>
@@ -5406,30 +5433,30 @@
         <v>14</v>
       </c>
       <c r="G98" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="H98" t="s">
         <v>14</v>
       </c>
       <c r="I98" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="J98" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B99" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C99" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D99" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E99" t="s">
         <v>14</v>
@@ -5438,30 +5465,30 @@
         <v>14</v>
       </c>
       <c r="G99" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="H99" t="s">
         <v>14</v>
       </c>
       <c r="I99" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="J99" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B100" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C100" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D100" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E100" t="s">
         <v>14</v>
@@ -5470,30 +5497,30 @@
         <v>14</v>
       </c>
       <c r="G100" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="H100" t="s">
         <v>14</v>
       </c>
       <c r="I100" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="J100" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B101" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C101" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D101" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E101" t="s">
         <v>14</v>
@@ -5502,30 +5529,30 @@
         <v>14</v>
       </c>
       <c r="G101" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="H101" t="s">
         <v>14</v>
       </c>
       <c r="I101" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="J101" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B102" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C102" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D102" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="E102" t="s">
         <v>14</v>
@@ -5534,62 +5561,62 @@
         <v>14</v>
       </c>
       <c r="G102" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="H102" t="s">
         <v>14</v>
       </c>
       <c r="I102" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="J102" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B103" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C103" t="s">
+        <v>559</v>
+      </c>
+      <c r="D103" t="s">
+        <v>555</v>
+      </c>
+      <c r="E103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F103" t="s">
+        <v>14</v>
+      </c>
+      <c r="G103" t="s">
+        <v>556</v>
+      </c>
+      <c r="H103" t="s">
+        <v>14</v>
+      </c>
+      <c r="I103" t="s">
+        <v>557</v>
+      </c>
+      <c r="J103" t="s">
         <v>558</v>
-      </c>
-      <c r="D103" t="s">
-        <v>554</v>
-      </c>
-      <c r="E103" t="s">
-        <v>14</v>
-      </c>
-      <c r="F103" t="s">
-        <v>14</v>
-      </c>
-      <c r="G103" t="s">
-        <v>555</v>
-      </c>
-      <c r="H103" t="s">
-        <v>14</v>
-      </c>
-      <c r="I103" t="s">
-        <v>556</v>
-      </c>
-      <c r="J103" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B104" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C104" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D104" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E104" t="s">
         <v>14</v>
@@ -5598,30 +5625,30 @@
         <v>14</v>
       </c>
       <c r="G104" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="H104" t="s">
         <v>14</v>
       </c>
       <c r="I104" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="J104" t="s">
-        <v>479</v>
+        <v>563</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="B105" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C105" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D105" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="E105" t="s">
         <v>14</v>
@@ -5630,30 +5657,30 @@
         <v>14</v>
       </c>
       <c r="G105" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="H105" t="s">
         <v>14</v>
       </c>
       <c r="I105" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="J105" t="s">
-        <v>479</v>
+        <v>568</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="B106" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="C106" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D106" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="E106" t="s">
         <v>14</v>
@@ -5662,30 +5689,30 @@
         <v>14</v>
       </c>
       <c r="G106" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="H106" t="s">
         <v>14</v>
       </c>
       <c r="I106" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="J106" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="B107" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C107" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D107" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="E107" t="s">
         <v>14</v>
@@ -5694,30 +5721,30 @@
         <v>14</v>
       </c>
       <c r="G107" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="H107" t="s">
         <v>14</v>
       </c>
       <c r="I107" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="J107" t="s">
-        <v>436</v>
+        <v>578</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="B108" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="C108" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D108" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="E108" t="s">
         <v>14</v>
@@ -5726,30 +5753,30 @@
         <v>14</v>
       </c>
       <c r="G108" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="H108" t="s">
         <v>14</v>
       </c>
       <c r="I108" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="J108" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="B109" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="C109" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D109" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="E109" t="s">
         <v>14</v>
@@ -5758,30 +5785,30 @@
         <v>14</v>
       </c>
       <c r="G109" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="H109" t="s">
         <v>14</v>
       </c>
       <c r="I109" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="J109" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="B110" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="C110" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D110" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
       <c r="E110" t="s">
         <v>14</v>
@@ -5790,30 +5817,30 @@
         <v>14</v>
       </c>
       <c r="G110" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="H110" t="s">
         <v>14</v>
       </c>
       <c r="I110" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="J110" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="B111" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C111" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D111" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="E111" t="s">
         <v>14</v>
@@ -5822,30 +5849,30 @@
         <v>14</v>
       </c>
       <c r="G111" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="H111" t="s">
         <v>14</v>
       </c>
       <c r="I111" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="J111" t="s">
-        <v>383</v>
+        <v>597</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="B112" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="C112" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D112" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="E112" t="s">
         <v>14</v>
@@ -5854,30 +5881,30 @@
         <v>14</v>
       </c>
       <c r="G112" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="H112" t="s">
         <v>14</v>
       </c>
       <c r="I112" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="J112" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="B113" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="C113" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D113" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="E113" t="s">
         <v>14</v>
@@ -5886,30 +5913,30 @@
         <v>14</v>
       </c>
       <c r="G113" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="H113" t="s">
         <v>14</v>
       </c>
       <c r="I113" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
       <c r="J113" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="B114" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C114" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D114" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="E114" t="s">
         <v>14</v>
@@ -5918,30 +5945,30 @@
         <v>14</v>
       </c>
       <c r="G114" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="H114" t="s">
         <v>14</v>
       </c>
       <c r="I114" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="J114" t="s">
-        <v>513</v>
+        <v>612</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="B115" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C115" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D115" t="s">
-        <v>607</v>
+        <v>613</v>
       </c>
       <c r="E115" t="s">
         <v>14</v>
@@ -5950,30 +5977,30 @@
         <v>14</v>
       </c>
       <c r="G115" t="s">
-        <v>608</v>
+        <v>614</v>
       </c>
       <c r="H115" t="s">
         <v>14</v>
       </c>
       <c r="I115" t="s">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="J115" t="s">
-        <v>485</v>
+        <v>616</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
       <c r="B116" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C116" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D116" t="s">
-        <v>611</v>
+        <v>618</v>
       </c>
       <c r="E116" t="s">
         <v>14</v>
@@ -5982,30 +6009,30 @@
         <v>14</v>
       </c>
       <c r="G116" t="s">
-        <v>612</v>
+        <v>619</v>
       </c>
       <c r="H116" t="s">
         <v>14</v>
       </c>
       <c r="I116" t="s">
-        <v>613</v>
+        <v>620</v>
       </c>
       <c r="J116" t="s">
-        <v>383</v>
+        <v>621</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
       <c r="B117" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
       <c r="C117" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D117" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="E117" t="s">
         <v>14</v>
@@ -6014,30 +6041,30 @@
         <v>14</v>
       </c>
       <c r="G117" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="H117" t="s">
         <v>14</v>
       </c>
       <c r="I117" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="J117" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
       <c r="B118" t="s">
-        <v>619</v>
+        <v>627</v>
       </c>
       <c r="C118" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D118" t="s">
-        <v>620</v>
+        <v>628</v>
       </c>
       <c r="E118" t="s">
         <v>14</v>
@@ -6046,30 +6073,30 @@
         <v>14</v>
       </c>
       <c r="G118" t="s">
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="H118" t="s">
         <v>14</v>
       </c>
       <c r="I118" t="s">
-        <v>622</v>
+        <v>630</v>
       </c>
       <c r="J118" t="s">
-        <v>623</v>
+        <v>631</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
       <c r="B119" t="s">
-        <v>624</v>
+        <v>632</v>
       </c>
       <c r="C119" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D119" t="s">
-        <v>625</v>
+        <v>633</v>
       </c>
       <c r="E119" t="s">
         <v>14</v>
@@ -6078,30 +6105,30 @@
         <v>14</v>
       </c>
       <c r="G119" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="H119" t="s">
         <v>14</v>
       </c>
       <c r="I119" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="J119" t="s">
-        <v>628</v>
+        <v>636</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
       <c r="B120" t="s">
-        <v>629</v>
+        <v>637</v>
       </c>
       <c r="C120" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D120" t="s">
-        <v>630</v>
+        <v>638</v>
       </c>
       <c r="E120" t="s">
         <v>14</v>
@@ -6110,30 +6137,30 @@
         <v>14</v>
       </c>
       <c r="G120" t="s">
-        <v>631</v>
+        <v>639</v>
       </c>
       <c r="H120" t="s">
         <v>14</v>
       </c>
       <c r="I120" t="s">
-        <v>632</v>
+        <v>640</v>
       </c>
       <c r="J120" t="s">
-        <v>633</v>
+        <v>641</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>634</v>
+        <v>642</v>
       </c>
       <c r="B121" t="s">
-        <v>635</v>
+        <v>643</v>
       </c>
       <c r="C121" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D121" t="s">
-        <v>636</v>
+        <v>644</v>
       </c>
       <c r="E121" t="s">
         <v>14</v>
@@ -6142,30 +6169,30 @@
         <v>14</v>
       </c>
       <c r="G121" t="s">
-        <v>637</v>
+        <v>645</v>
       </c>
       <c r="H121" t="s">
         <v>14</v>
       </c>
       <c r="I121" t="s">
-        <v>638</v>
+        <v>646</v>
       </c>
       <c r="J121" t="s">
-        <v>639</v>
+        <v>647</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>634</v>
+        <v>642</v>
       </c>
       <c r="B122" t="s">
-        <v>640</v>
+        <v>648</v>
       </c>
       <c r="C122" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D122" t="s">
-        <v>641</v>
+        <v>649</v>
       </c>
       <c r="E122" t="s">
         <v>14</v>
@@ -6174,30 +6201,30 @@
         <v>14</v>
       </c>
       <c r="G122" t="s">
-        <v>642</v>
+        <v>650</v>
       </c>
       <c r="H122" t="s">
         <v>14</v>
       </c>
       <c r="I122" t="s">
-        <v>643</v>
+        <v>651</v>
       </c>
       <c r="J122" t="s">
-        <v>644</v>
+        <v>652</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>634</v>
+        <v>642</v>
       </c>
       <c r="B123" t="s">
-        <v>645</v>
+        <v>653</v>
       </c>
       <c r="C123" t="s">
-        <v>645</v>
+        <v>653</v>
       </c>
       <c r="D123" t="s">
-        <v>646</v>
+        <v>654</v>
       </c>
       <c r="E123" t="s">
         <v>14</v>
@@ -6206,27 +6233,27 @@
         <v>14</v>
       </c>
       <c r="G123" t="s">
-        <v>647</v>
+        <v>655</v>
       </c>
       <c r="H123" t="s">
         <v>14</v>
       </c>
       <c r="I123" t="s">
-        <v>648</v>
+        <v>656</v>
       </c>
       <c r="J123" t="s">
-        <v>649</v>
+        <v>657</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>634</v>
+        <v>642</v>
       </c>
       <c r="B124" t="s">
-        <v>645</v>
+        <v>653</v>
       </c>
       <c r="D124" t="s">
-        <v>650</v>
+        <v>658</v>
       </c>
       <c r="E124" t="s">
         <v>14</v>
@@ -6235,16 +6262,16 @@
         <v>14</v>
       </c>
       <c r="G124" t="s">
-        <v>651</v>
+        <v>659</v>
       </c>
       <c r="H124" t="s">
         <v>14</v>
       </c>
       <c r="I124" t="s">
-        <v>652</v>
+        <v>660</v>
       </c>
       <c r="J124" t="s">
-        <v>649</v>
+        <v>661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>